<commit_message>
Actualizando alcance del sistema
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="114">
   <si>
     <t>Persona</t>
   </si>
@@ -219,9 +219,6 @@
     <t>teresa@mail.com</t>
   </si>
   <si>
-    <t>emilio@mail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">VAIRA                                             </t>
   </si>
   <si>
@@ -273,12 +270,6 @@
     <t>aide@mail.com</t>
   </si>
   <si>
-    <t>amada@mail.com</t>
-  </si>
-  <si>
-    <t>eduardo@mail.com</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
@@ -346,6 +337,27 @@
   </si>
   <si>
     <t>Acordar con el vendedor</t>
+  </si>
+  <si>
+    <t>DetallePedido</t>
+  </si>
+  <si>
+    <t>[Cantidad]</t>
+  </si>
+  <si>
+    <t>TipoPersona</t>
+  </si>
+  <si>
+    <t>Fisica</t>
+  </si>
+  <si>
+    <t>Juridica</t>
+  </si>
+  <si>
+    <t>Preparado</t>
+  </si>
+  <si>
+    <t>Cancelado</t>
   </si>
 </sst>
 </file>
@@ -800,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:O79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -821,7 +833,7 @@
     <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -834,7 +846,7 @@
       </c>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -857,7 +869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -877,7 +889,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -897,7 +909,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -914,10 +926,10 @@
         <v>3</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -931,7 +943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -941,10 +953,12 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="I8" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -964,16 +978,16 @@
         <v>34</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="I9" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="13">
         <v>1</v>
       </c>
@@ -986,14 +1000,15 @@
       <c r="D10" s="16">
         <v>6781261</v>
       </c>
-      <c r="G10" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="16">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="G10" s="16"/>
+      <c r="I10" s="18">
+        <v>1</v>
+      </c>
+      <c r="J10" s="19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="13">
         <v>2</v>
       </c>
@@ -1006,14 +1021,15 @@
       <c r="D11" s="16">
         <v>6815325</v>
       </c>
-      <c r="G11" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="16">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="G11" s="16"/>
+      <c r="I11" s="18">
+        <v>2</v>
+      </c>
+      <c r="J11" s="19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="13">
         <v>3</v>
       </c>
@@ -1026,14 +1042,9 @@
       <c r="D12" s="16">
         <v>6803235</v>
       </c>
-      <c r="G12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="16">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="13">
         <v>4</v>
       </c>
@@ -1046,14 +1057,9 @@
       <c r="D13" s="16">
         <v>6800553</v>
       </c>
-      <c r="G13" t="s">
-        <v>65</v>
-      </c>
-      <c r="H13" s="16">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="13">
         <v>5</v>
       </c>
@@ -1066,14 +1072,9 @@
       <c r="D14" s="16">
         <v>792947</v>
       </c>
-      <c r="G14" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="16">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="G14" s="16"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="13">
         <v>6</v>
       </c>
@@ -1086,172 +1087,127 @@
       <c r="D15" s="16">
         <v>6801988</v>
       </c>
-      <c r="G15" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="16">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="13">
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="G16" t="s">
-        <v>98</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>81</v>
-      </c>
+      <c r="G16" s="16"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="13">
         <v>8</v>
       </c>
       <c r="B17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="C17" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="G17" t="s">
-        <v>99</v>
-      </c>
-      <c r="H17" s="16" t="s">
-        <v>81</v>
-      </c>
+      <c r="G17" s="16"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="13">
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="G18" t="s">
-        <v>100</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>81</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="G18" s="16"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="13">
         <v>10</v>
       </c>
       <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" t="s">
         <v>68</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" t="s">
-        <v>82</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>81</v>
-      </c>
+      <c r="G19" s="16"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="13">
         <v>11</v>
       </c>
       <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
         <v>71</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="G20" t="s">
-        <v>83</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>81</v>
-      </c>
+      <c r="G20" s="16"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="13">
         <v>12</v>
       </c>
       <c r="B21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" t="s">
         <v>74</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21" t="s">
-        <v>84</v>
-      </c>
-      <c r="H21" s="16" t="s">
-        <v>81</v>
-      </c>
+      <c r="G21" s="16"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="13">
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="G22" t="s">
-        <v>85</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>81</v>
-      </c>
+      <c r="G22" s="16"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="13">
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="G23" t="s">
-        <v>86</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>81</v>
-      </c>
+      <c r="G23" s="16"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="13"/>
@@ -1264,14 +1220,13 @@
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
-      <c r="E26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="I26" s="3" t="s">
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="G26" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
     </row>
@@ -1283,22 +1238,25 @@
         <v>4</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F27" s="4" t="s">
+      <c r="G27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="I27" s="4" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>15</v>
@@ -1311,26 +1269,29 @@
       <c r="B28" s="13">
         <v>10</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E28" s="13">
-        <v>1</v>
-      </c>
-      <c r="F28" s="13">
-        <v>7</v>
-      </c>
-      <c r="G28" t="s">
-        <v>87</v>
-      </c>
-      <c r="I28" s="13">
-        <v>1</v>
-      </c>
-      <c r="J28" s="13">
-        <v>1</v>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G28" s="13">
+        <v>1</v>
+      </c>
+      <c r="H28" s="13">
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>62</v>
+      </c>
+      <c r="J28" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="K28" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1340,26 +1301,29 @@
       <c r="B29" s="13">
         <v>11</v>
       </c>
-      <c r="C29" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="13">
-        <v>2</v>
-      </c>
-      <c r="F29" s="13">
-        <v>8</v>
-      </c>
-      <c r="G29" t="s">
-        <v>87</v>
-      </c>
-      <c r="I29" s="13">
-        <v>2</v>
-      </c>
-      <c r="J29" s="13">
-        <v>2</v>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G29" s="13">
+        <v>2</v>
+      </c>
+      <c r="H29" s="13">
+        <v>2</v>
+      </c>
+      <c r="I29" t="s">
+        <v>63</v>
+      </c>
+      <c r="J29" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="K29" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1369,26 +1333,29 @@
       <c r="B30" s="13">
         <v>12</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E30" s="13">
+      <c r="C30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G30" s="13">
         <v>3</v>
       </c>
-      <c r="F30" s="13">
-        <v>9</v>
-      </c>
-      <c r="G30" t="s">
-        <v>87</v>
-      </c>
-      <c r="I30" s="13">
+      <c r="H30" s="13">
         <v>3</v>
       </c>
-      <c r="J30" s="13">
-        <v>3</v>
+      <c r="I30" t="s">
+        <v>64</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="K30" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1397,14 +1364,20 @@
       <c r="C31" s="13"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
-      <c r="I31" s="13">
+      <c r="G31" s="13">
         <v>4</v>
       </c>
-      <c r="J31" s="13">
-        <v>8</v>
+      <c r="H31" s="13">
+        <v>4</v>
+      </c>
+      <c r="I31" t="s">
+        <v>65</v>
+      </c>
+      <c r="J31" s="16">
+        <v>123</v>
       </c>
       <c r="K31" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1413,395 +1386,600 @@
       <c r="C32" s="13"/>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
-      <c r="I32" s="13">
+      <c r="G32" s="13">
         <v>5</v>
       </c>
-      <c r="J32" s="13">
-        <v>14</v>
+      <c r="H32" s="13">
+        <v>5</v>
+      </c>
+      <c r="I32" t="s">
+        <v>66</v>
+      </c>
+      <c r="J32" s="16">
+        <v>123</v>
       </c>
       <c r="K32" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="6" t="s">
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="13">
+        <v>1</v>
+      </c>
+      <c r="B36" s="13">
         <v>7</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="C36" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" t="s">
+        <v>84</v>
+      </c>
+      <c r="F36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="13">
+        <v>2</v>
+      </c>
+      <c r="B37" s="13">
         <v>8</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="13">
-        <v>1</v>
-      </c>
-      <c r="C36" s="13">
-        <v>1</v>
-      </c>
-      <c r="E36">
-        <v>10</v>
-      </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="H36" t="s">
-        <v>87</v>
-      </c>
-      <c r="I36" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="13">
-        <v>2</v>
-      </c>
-      <c r="C37" s="13">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>15</v>
-      </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="H37" t="s">
-        <v>87</v>
-      </c>
-      <c r="I37" s="13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+      <c r="C37" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" t="s">
+        <v>84</v>
+      </c>
+      <c r="F37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="13">
         <v>3</v>
       </c>
-      <c r="C38" s="13">
-        <v>2</v>
-      </c>
-      <c r="E38">
-        <v>20</v>
-      </c>
-      <c r="F38">
-        <v>1</v>
-      </c>
-      <c r="H38" t="s">
-        <v>87</v>
-      </c>
-      <c r="I38" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="13">
-        <v>4</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="D39" t="s">
-        <v>103</v>
-      </c>
-      <c r="E39">
-        <v>30</v>
-      </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-      <c r="G39" t="s">
-        <v>104</v>
-      </c>
-      <c r="H39" t="s">
-        <v>87</v>
-      </c>
-      <c r="I39" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="13">
-        <v>5</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="D40" t="s">
-        <v>102</v>
-      </c>
-      <c r="E40">
-        <v>40</v>
-      </c>
-      <c r="F40">
-        <v>1</v>
-      </c>
-      <c r="G40" t="s">
-        <v>105</v>
-      </c>
-      <c r="H40" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="I40" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="13">
-        <v>6</v>
-      </c>
-      <c r="C41" s="13">
-        <v>2</v>
-      </c>
-      <c r="E41">
-        <v>50</v>
-      </c>
-      <c r="F41">
-        <v>1</v>
-      </c>
-      <c r="G41" s="12"/>
-      <c r="H41" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="I41" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="13">
-        <v>7</v>
-      </c>
-      <c r="C42" s="13">
-        <v>3</v>
-      </c>
-      <c r="E42">
-        <v>60</v>
-      </c>
-      <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="G42" s="12"/>
-      <c r="H42" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="I42" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="13">
-        <v>8</v>
-      </c>
-      <c r="C43" s="13">
-        <v>4</v>
-      </c>
-      <c r="E43">
-        <v>70</v>
-      </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-      <c r="G43" s="12"/>
-      <c r="H43" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="I43" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+      <c r="B38" s="13">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E38" t="s">
+        <v>84</v>
+      </c>
+      <c r="F38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="13"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="13"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="13"/>
-    </row>
-    <row r="50" spans="1:15">
-      <c r="A50" s="7" t="s">
+      <c r="C44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="13">
+        <v>1</v>
+      </c>
+      <c r="C48" s="13">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>10</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="H48" t="s">
+        <v>84</v>
+      </c>
+      <c r="I48" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="13">
+        <v>2</v>
+      </c>
+      <c r="C49" s="13">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>15</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="H49" t="s">
+        <v>84</v>
+      </c>
+      <c r="I49" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="13">
+        <v>3</v>
+      </c>
+      <c r="C50" s="13">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>20</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="H50" t="s">
+        <v>84</v>
+      </c>
+      <c r="I50" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="13">
+        <v>4</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51" t="s">
+        <v>100</v>
+      </c>
+      <c r="E51">
+        <v>30</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51" t="s">
+        <v>101</v>
+      </c>
+      <c r="H51" t="s">
+        <v>84</v>
+      </c>
+      <c r="I51" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="13">
+        <v>5</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" t="s">
+        <v>99</v>
+      </c>
+      <c r="E52">
+        <v>40</v>
+      </c>
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52" t="s">
+        <v>102</v>
+      </c>
+      <c r="H52" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I52" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="13">
+        <v>6</v>
+      </c>
+      <c r="C53" s="13">
+        <v>2</v>
+      </c>
+      <c r="E53">
+        <v>50</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53" s="12"/>
+      <c r="H53" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I53" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="13">
+        <v>7</v>
+      </c>
+      <c r="C54" s="13">
+        <v>3</v>
+      </c>
+      <c r="E54">
+        <v>60</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54" s="12"/>
+      <c r="H54" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I54" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="13">
+        <v>8</v>
+      </c>
+      <c r="C55" s="13">
+        <v>4</v>
+      </c>
+      <c r="E55">
+        <v>70</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55" s="12"/>
+      <c r="H55" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="I55" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="13"/>
+      <c r="B56" s="13"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="13"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="13"/>
+      <c r="B57" s="13"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="13"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="13"/>
+      <c r="B58" s="13"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="13"/>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="13"/>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F60" s="12"/>
+      <c r="G60" s="13"/>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="13"/>
+    </row>
+    <row r="65" spans="1:15">
+      <c r="A65" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="N50" s="20"/>
-      <c r="O50" s="21"/>
-    </row>
-    <row r="51" spans="1:15">
-      <c r="A51" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B51" s="8" t="s">
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8"/>
+      <c r="F65" s="8"/>
+      <c r="G65" s="8"/>
+      <c r="N65" s="20"/>
+      <c r="O65" s="21"/>
+    </row>
+    <row r="66" spans="1:15">
+      <c r="A66" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C51" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" s="8" t="s">
+      <c r="C66" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F51" s="8" t="s">
+      <c r="D66" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E66" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G66" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N66" s="20"/>
+      <c r="O66" s="21"/>
+    </row>
+    <row r="67" spans="1:15">
+      <c r="N67" s="20"/>
+      <c r="O67" s="21"/>
+    </row>
+    <row r="68" spans="1:15">
+      <c r="N68" s="20"/>
+      <c r="O68" s="21"/>
+    </row>
+    <row r="69" spans="1:15">
+      <c r="N69" s="20"/>
+      <c r="O69" s="21"/>
+    </row>
+    <row r="70" spans="1:15">
+      <c r="A70" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70" s="10"/>
+      <c r="D70" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E70" s="10"/>
+      <c r="M70" s="13"/>
+      <c r="N70" s="14"/>
+    </row>
+    <row r="71" spans="1:15">
+      <c r="A71" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15">
+      <c r="A72" s="18">
+        <v>1</v>
+      </c>
+      <c r="B72" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D72" s="13">
+        <v>1</v>
+      </c>
+      <c r="E72" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15">
+      <c r="A73" s="18">
+        <v>2</v>
+      </c>
+      <c r="B73" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D73" s="13">
+        <v>2</v>
+      </c>
+      <c r="E73" t="s">
         <v>106</v>
       </c>
-      <c r="G51" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H51" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I51" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N51" s="20"/>
-      <c r="O51" s="21"/>
-    </row>
-    <row r="52" spans="1:15">
-      <c r="N52" s="20"/>
-      <c r="O52" s="21"/>
-    </row>
-    <row r="53" spans="1:15">
-      <c r="N53" s="20"/>
-      <c r="O53" s="21"/>
-    </row>
-    <row r="54" spans="1:15">
-      <c r="N54" s="20"/>
-      <c r="O54" s="21"/>
-    </row>
-    <row r="55" spans="1:15">
-      <c r="A55" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B55" s="10"/>
-      <c r="D55" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E55" s="10"/>
-      <c r="M55" s="13"/>
-      <c r="N55" s="14"/>
-    </row>
-    <row r="56" spans="1:15">
-      <c r="A56" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B56" s="10" t="s">
+    </row>
+    <row r="74" spans="1:15">
+      <c r="A74" s="18">
+        <v>2</v>
+      </c>
+      <c r="B74" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
+      <c r="A75" s="18">
         <v>3</v>
       </c>
-      <c r="D56" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15">
-      <c r="A57" s="18">
-        <v>1</v>
-      </c>
-      <c r="B57" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D57" s="13">
-        <v>1</v>
-      </c>
-      <c r="E57" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15">
-      <c r="A58" s="18">
-        <v>2</v>
-      </c>
-      <c r="B58" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D58" s="13">
-        <v>2</v>
-      </c>
-      <c r="E58" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15">
-      <c r="A59" s="18">
-        <v>3</v>
-      </c>
-      <c r="B59" s="19" t="s">
+      <c r="B75" s="19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
-      <c r="A62" s="22" t="s">
+    <row r="76" spans="1:15">
+      <c r="A76" s="18">
+        <v>4</v>
+      </c>
+      <c r="B76" s="19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15">
+      <c r="A78" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
-    </row>
-    <row r="63" spans="1:15">
-      <c r="A63" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B63" s="11" t="s">
+      <c r="B78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+    </row>
+    <row r="79" spans="1:15">
+      <c r="A79" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B79" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="C79" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D63" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E63" s="11" t="s">
+      <c r="D79" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E79" s="11" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>